<commit_message>
Updated ec, crushmap and bgp
</commit_message>
<xml_diff>
--- a/cookbooks/chef-bcs/files/default/utilities/BCS-Erasure-Coding-Calcs.xlsx
+++ b/cookbooks/chef-bcs/files/default/utilities/BCS-Erasure-Coding-Calcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21760" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21760" windowHeight="20460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Green - Input values</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Note: Ceph itself will take up some space so the numbers above will be a little less that what's displayed. Use 'ceph df' once installed to see available and max available.</t>
+  </si>
+  <si>
+    <t>Full Ratio</t>
   </si>
 </sst>
 </file>
@@ -185,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -289,8 +292,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -343,8 +355,92 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -393,44 +489,56 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="46">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -440,6 +548,20 @@
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -448,6 +570,20 @@
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1768,13 +1904,13 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IR29"/>
+  <dimension ref="A1:IS34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -1783,442 +1919,2134 @@
     <col min="2" max="2" width="11.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="1" customWidth="1"/>
     <col min="4" max="5" width="11.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.375" style="1" customWidth="1"/>
-    <col min="7" max="252" width="9" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="12.375" style="1" customWidth="1"/>
+    <col min="8" max="253" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31" customHeight="1">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:253" ht="31" customHeight="1">
+      <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
-    <row r="2" spans="1:6" ht="27" customHeight="1">
+    <row r="2" spans="1:253" ht="27" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="13">
-        <v>1000</v>
+        <v>612</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="9">
-        <f>+B2*B3</f>
-        <v>6000</v>
-      </c>
-      <c r="F2" s="16"/>
+        <f>+B2*B4</f>
+        <v>3672</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="18"/>
     </row>
-    <row r="3" spans="1:6" ht="24" customHeight="1">
+    <row r="3" spans="1:253" ht="27" customHeight="1">
       <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="31">
+        <v>0.95</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="20"/>
+      <c r="Y3" s="20"/>
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="20"/>
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
+      <c r="AG3" s="20"/>
+      <c r="AH3" s="20"/>
+      <c r="AI3" s="20"/>
+      <c r="AJ3" s="20"/>
+      <c r="AK3" s="20"/>
+      <c r="AL3" s="20"/>
+      <c r="AM3" s="20"/>
+      <c r="AN3" s="20"/>
+      <c r="AO3" s="20"/>
+      <c r="AP3" s="20"/>
+      <c r="AQ3" s="20"/>
+      <c r="AR3" s="20"/>
+      <c r="AS3" s="20"/>
+      <c r="AT3" s="20"/>
+      <c r="AU3" s="20"/>
+      <c r="AV3" s="20"/>
+      <c r="AW3" s="20"/>
+      <c r="AX3" s="20"/>
+      <c r="AY3" s="20"/>
+      <c r="AZ3" s="20"/>
+      <c r="BA3" s="20"/>
+      <c r="BB3" s="20"/>
+      <c r="BC3" s="20"/>
+      <c r="BD3" s="20"/>
+      <c r="BE3" s="20"/>
+      <c r="BF3" s="20"/>
+      <c r="BG3" s="20"/>
+      <c r="BH3" s="20"/>
+      <c r="BI3" s="20"/>
+      <c r="BJ3" s="20"/>
+      <c r="BK3" s="20"/>
+      <c r="BL3" s="20"/>
+      <c r="BM3" s="20"/>
+      <c r="BN3" s="20"/>
+      <c r="BO3" s="20"/>
+      <c r="BP3" s="20"/>
+      <c r="BQ3" s="20"/>
+      <c r="BR3" s="20"/>
+      <c r="BS3" s="20"/>
+      <c r="BT3" s="20"/>
+      <c r="BU3" s="20"/>
+      <c r="BV3" s="20"/>
+      <c r="BW3" s="20"/>
+      <c r="BX3" s="20"/>
+      <c r="BY3" s="20"/>
+      <c r="BZ3" s="20"/>
+      <c r="CA3" s="20"/>
+      <c r="CB3" s="20"/>
+      <c r="CC3" s="20"/>
+      <c r="CD3" s="20"/>
+      <c r="CE3" s="20"/>
+      <c r="CF3" s="20"/>
+      <c r="CG3" s="20"/>
+      <c r="CH3" s="20"/>
+      <c r="CI3" s="20"/>
+      <c r="CJ3" s="20"/>
+      <c r="CK3" s="20"/>
+      <c r="CL3" s="20"/>
+      <c r="CM3" s="20"/>
+      <c r="CN3" s="20"/>
+      <c r="CO3" s="20"/>
+      <c r="CP3" s="20"/>
+      <c r="CQ3" s="20"/>
+      <c r="CR3" s="20"/>
+      <c r="CS3" s="20"/>
+      <c r="CT3" s="20"/>
+      <c r="CU3" s="20"/>
+      <c r="CV3" s="20"/>
+      <c r="CW3" s="20"/>
+      <c r="CX3" s="20"/>
+      <c r="CY3" s="20"/>
+      <c r="CZ3" s="20"/>
+      <c r="DA3" s="20"/>
+      <c r="DB3" s="20"/>
+      <c r="DC3" s="20"/>
+      <c r="DD3" s="20"/>
+      <c r="DE3" s="20"/>
+      <c r="DF3" s="20"/>
+      <c r="DG3" s="20"/>
+      <c r="DH3" s="20"/>
+      <c r="DI3" s="20"/>
+      <c r="DJ3" s="20"/>
+      <c r="DK3" s="20"/>
+      <c r="DL3" s="20"/>
+      <c r="DM3" s="20"/>
+      <c r="DN3" s="20"/>
+      <c r="DO3" s="20"/>
+      <c r="DP3" s="20"/>
+      <c r="DQ3" s="20"/>
+      <c r="DR3" s="20"/>
+      <c r="DS3" s="20"/>
+      <c r="DT3" s="20"/>
+      <c r="DU3" s="20"/>
+      <c r="DV3" s="20"/>
+      <c r="DW3" s="20"/>
+      <c r="DX3" s="20"/>
+      <c r="DY3" s="20"/>
+      <c r="DZ3" s="20"/>
+      <c r="EA3" s="20"/>
+      <c r="EB3" s="20"/>
+      <c r="EC3" s="20"/>
+      <c r="ED3" s="20"/>
+      <c r="EE3" s="20"/>
+      <c r="EF3" s="20"/>
+      <c r="EG3" s="20"/>
+      <c r="EH3" s="20"/>
+      <c r="EI3" s="20"/>
+      <c r="EJ3" s="20"/>
+      <c r="EK3" s="20"/>
+      <c r="EL3" s="20"/>
+      <c r="EM3" s="20"/>
+      <c r="EN3" s="20"/>
+      <c r="EO3" s="20"/>
+      <c r="EP3" s="20"/>
+      <c r="EQ3" s="20"/>
+      <c r="ER3" s="20"/>
+      <c r="ES3" s="20"/>
+      <c r="ET3" s="20"/>
+      <c r="EU3" s="20"/>
+      <c r="EV3" s="20"/>
+      <c r="EW3" s="20"/>
+      <c r="EX3" s="20"/>
+      <c r="EY3" s="20"/>
+      <c r="EZ3" s="20"/>
+      <c r="FA3" s="20"/>
+      <c r="FB3" s="20"/>
+      <c r="FC3" s="20"/>
+      <c r="FD3" s="20"/>
+      <c r="FE3" s="20"/>
+      <c r="FF3" s="20"/>
+      <c r="FG3" s="20"/>
+      <c r="FH3" s="20"/>
+      <c r="FI3" s="20"/>
+      <c r="FJ3" s="20"/>
+      <c r="FK3" s="20"/>
+      <c r="FL3" s="20"/>
+      <c r="FM3" s="20"/>
+      <c r="FN3" s="20"/>
+      <c r="FO3" s="20"/>
+      <c r="FP3" s="20"/>
+      <c r="FQ3" s="20"/>
+      <c r="FR3" s="20"/>
+      <c r="FS3" s="20"/>
+      <c r="FT3" s="20"/>
+      <c r="FU3" s="20"/>
+      <c r="FV3" s="20"/>
+      <c r="FW3" s="20"/>
+      <c r="FX3" s="20"/>
+      <c r="FY3" s="20"/>
+      <c r="FZ3" s="20"/>
+      <c r="GA3" s="20"/>
+      <c r="GB3" s="20"/>
+      <c r="GC3" s="20"/>
+      <c r="GD3" s="20"/>
+      <c r="GE3" s="20"/>
+      <c r="GF3" s="20"/>
+      <c r="GG3" s="20"/>
+      <c r="GH3" s="20"/>
+      <c r="GI3" s="20"/>
+      <c r="GJ3" s="20"/>
+      <c r="GK3" s="20"/>
+      <c r="GL3" s="20"/>
+      <c r="GM3" s="20"/>
+      <c r="GN3" s="20"/>
+      <c r="GO3" s="20"/>
+      <c r="GP3" s="20"/>
+      <c r="GQ3" s="20"/>
+      <c r="GR3" s="20"/>
+      <c r="GS3" s="20"/>
+      <c r="GT3" s="20"/>
+      <c r="GU3" s="20"/>
+      <c r="GV3" s="20"/>
+      <c r="GW3" s="20"/>
+      <c r="GX3" s="20"/>
+      <c r="GY3" s="20"/>
+      <c r="GZ3" s="20"/>
+      <c r="HA3" s="20"/>
+      <c r="HB3" s="20"/>
+      <c r="HC3" s="20"/>
+      <c r="HD3" s="20"/>
+      <c r="HE3" s="20"/>
+      <c r="HF3" s="20"/>
+      <c r="HG3" s="20"/>
+      <c r="HH3" s="20"/>
+      <c r="HI3" s="20"/>
+      <c r="HJ3" s="20"/>
+      <c r="HK3" s="20"/>
+      <c r="HL3" s="20"/>
+      <c r="HM3" s="20"/>
+      <c r="HN3" s="20"/>
+      <c r="HO3" s="20"/>
+      <c r="HP3" s="20"/>
+      <c r="HQ3" s="20"/>
+      <c r="HR3" s="20"/>
+      <c r="HS3" s="20"/>
+      <c r="HT3" s="20"/>
+      <c r="HU3" s="20"/>
+      <c r="HV3" s="20"/>
+      <c r="HW3" s="20"/>
+      <c r="HX3" s="20"/>
+      <c r="HY3" s="20"/>
+      <c r="HZ3" s="20"/>
+      <c r="IA3" s="20"/>
+      <c r="IB3" s="20"/>
+      <c r="IC3" s="20"/>
+      <c r="ID3" s="20"/>
+      <c r="IE3" s="20"/>
+      <c r="IF3" s="20"/>
+      <c r="IG3" s="20"/>
+      <c r="IH3" s="20"/>
+      <c r="II3" s="20"/>
+      <c r="IJ3" s="20"/>
+      <c r="IK3" s="20"/>
+      <c r="IL3" s="20"/>
+      <c r="IM3" s="20"/>
+      <c r="IN3" s="20"/>
+      <c r="IO3" s="20"/>
+      <c r="IP3" s="20"/>
+      <c r="IQ3" s="20"/>
+      <c r="IR3" s="20"/>
+      <c r="IS3" s="20"/>
+    </row>
+    <row r="4" spans="1:253" ht="24" customHeight="1">
+      <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B4" s="14">
         <v>6</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="17"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="19"/>
     </row>
-    <row r="4" spans="1:6" ht="20.5" customHeight="1">
-      <c r="A4" s="15" t="s">
+    <row r="5" spans="1:253" ht="20.5" customHeight="1">
+      <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B5" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="27"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
-    <row r="5" spans="1:6" ht="28" customHeight="1">
-      <c r="A5" s="4" t="s">
+    <row r="6" spans="1:253" ht="28" customHeight="1">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B6" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C6" s="6">
         <v>2</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D6" s="6">
         <v>3</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E6" s="6">
         <v>4</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F6" s="6">
         <v>5</v>
       </c>
+      <c r="G6" s="6">
+        <v>6</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" ht="28" customHeight="1">
-      <c r="A6" s="3">
+    <row r="7" spans="1:253" ht="28" customHeight="1">
+      <c r="A7" s="3">
         <v>1</v>
       </c>
-      <c r="B6" s="10">
-        <f>+($B$2*$A6/($A6+B$5))*$B$3</f>
-        <v>3000</v>
-      </c>
-      <c r="C6" s="10">
-        <f t="shared" ref="C6:F15" si="0">+($B$2*$A6/($A6+C$5))*$B$3</f>
-        <v>2000</v>
-      </c>
-      <c r="D6" s="10">
-        <f t="shared" si="0"/>
-        <v>1500</v>
-      </c>
-      <c r="E6" s="10">
-        <f t="shared" si="0"/>
-        <v>1200</v>
-      </c>
-      <c r="F6" s="11">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+      <c r="B7" s="10">
+        <f>+($B$2*$A7/($A7+B$6))*$B$4*$B$3</f>
+        <v>1744.1999999999998</v>
+      </c>
+      <c r="C7" s="10">
+        <f t="shared" ref="C7:G21" si="0">+($B$2*$A7/($A7+C$6))*$B$4*$B$3</f>
+        <v>1162.8</v>
+      </c>
+      <c r="D7" s="10">
+        <f t="shared" si="0"/>
+        <v>872.09999999999991</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" si="0"/>
+        <v>697.68000000000006</v>
+      </c>
+      <c r="F7" s="10">
+        <f t="shared" si="0"/>
+        <v>581.4</v>
+      </c>
+      <c r="G7" s="11">
+        <f t="shared" si="0"/>
+        <v>498.3428571428571</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="32" customHeight="1">
-      <c r="A7" s="3">
+    <row r="8" spans="1:253" ht="32" customHeight="1">
+      <c r="A8" s="3">
         <v>2</v>
       </c>
-      <c r="B7" s="10">
-        <f t="shared" ref="B7:B15" si="1">+($B$2*$A7/($A7+B$5))*$B$3</f>
-        <v>4000</v>
-      </c>
-      <c r="C7" s="10">
-        <f t="shared" si="0"/>
-        <v>3000</v>
-      </c>
-      <c r="D7" s="10">
-        <f t="shared" si="0"/>
-        <v>2400</v>
-      </c>
-      <c r="E7" s="10">
-        <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-      <c r="F7" s="11">
-        <f t="shared" si="0"/>
-        <v>1714.2857142857142</v>
+      <c r="B8" s="10">
+        <f t="shared" ref="B8:B21" si="1">+($B$2*$A8/($A8+B$6))*$B$4*$B$3</f>
+        <v>2325.6</v>
+      </c>
+      <c r="C8" s="10">
+        <f t="shared" si="0"/>
+        <v>1744.1999999999998</v>
+      </c>
+      <c r="D8" s="10">
+        <f t="shared" si="0"/>
+        <v>1395.3600000000001</v>
+      </c>
+      <c r="E8" s="10">
+        <f t="shared" si="0"/>
+        <v>1162.8</v>
+      </c>
+      <c r="F8" s="10">
+        <f t="shared" si="0"/>
+        <v>996.6857142857142</v>
+      </c>
+      <c r="G8" s="11">
+        <f t="shared" si="0"/>
+        <v>872.09999999999991</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="31" customHeight="1">
-      <c r="A8" s="3">
+    <row r="9" spans="1:253" ht="31" customHeight="1">
+      <c r="A9" s="3">
         <v>3</v>
-      </c>
-      <c r="B8" s="10">
-        <f t="shared" si="1"/>
-        <v>4500</v>
-      </c>
-      <c r="C8" s="10">
-        <f t="shared" si="0"/>
-        <v>3600</v>
-      </c>
-      <c r="D8" s="10">
-        <f t="shared" si="0"/>
-        <v>3000</v>
-      </c>
-      <c r="E8" s="10">
-        <f t="shared" si="0"/>
-        <v>2571.4285714285716</v>
-      </c>
-      <c r="F8" s="11">
-        <f t="shared" si="0"/>
-        <v>2250</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A9" s="3">
-        <v>4</v>
       </c>
       <c r="B9" s="10">
         <f t="shared" si="1"/>
-        <v>4800</v>
+        <v>2616.2999999999997</v>
       </c>
       <c r="C9" s="10">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>2093.0399999999995</v>
       </c>
       <c r="D9" s="10">
         <f t="shared" si="0"/>
-        <v>3428.5714285714284</v>
+        <v>1744.1999999999998</v>
       </c>
       <c r="E9" s="10">
         <f t="shared" si="0"/>
-        <v>3000</v>
-      </c>
-      <c r="F9" s="11">
-        <f t="shared" si="0"/>
-        <v>2666.666666666667</v>
+        <v>1495.0285714285715</v>
+      </c>
+      <c r="F9" s="10">
+        <f t="shared" si="0"/>
+        <v>1308.1499999999999</v>
+      </c>
+      <c r="G9" s="11">
+        <f t="shared" si="0"/>
+        <v>1162.8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="32.25" customHeight="1">
+    <row r="10" spans="1:253" ht="32.25" customHeight="1">
       <c r="A10" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="10">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>2790.7200000000003</v>
       </c>
       <c r="C10" s="10">
         <f t="shared" si="0"/>
-        <v>4285.7142857142862</v>
+        <v>2325.6</v>
       </c>
       <c r="D10" s="10">
         <f t="shared" si="0"/>
-        <v>3750</v>
+        <v>1993.3714285714284</v>
       </c>
       <c r="E10" s="10">
         <f t="shared" si="0"/>
-        <v>3333.333333333333</v>
-      </c>
-      <c r="F10" s="11">
-        <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>1744.1999999999998</v>
+      </c>
+      <c r="F10" s="10">
+        <f t="shared" si="0"/>
+        <v>1550.3999999999999</v>
+      </c>
+      <c r="G10" s="11">
+        <f t="shared" si="0"/>
+        <v>1395.3600000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="32.25" customHeight="1">
+    <row r="11" spans="1:253" ht="32.25" customHeight="1">
       <c r="A11" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="10">
         <f t="shared" si="1"/>
-        <v>5142.8571428571431</v>
+        <v>2907</v>
       </c>
       <c r="C11" s="10">
         <f t="shared" si="0"/>
-        <v>4500</v>
+        <v>2491.7142857142858</v>
       </c>
       <c r="D11" s="10">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>2180.25</v>
       </c>
       <c r="E11" s="10">
         <f t="shared" si="0"/>
-        <v>3600</v>
-      </c>
-      <c r="F11" s="11">
-        <f t="shared" si="0"/>
-        <v>3272.727272727273</v>
+        <v>1938</v>
+      </c>
+      <c r="F11" s="10">
+        <f t="shared" si="0"/>
+        <v>1744.1999999999998</v>
+      </c>
+      <c r="G11" s="11">
+        <f t="shared" si="0"/>
+        <v>1585.6363636363635</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="32.25" customHeight="1">
+    <row r="12" spans="1:253" ht="32.25" customHeight="1">
       <c r="A12" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="10">
         <f t="shared" si="1"/>
-        <v>5250</v>
+        <v>2990.0571428571429</v>
       </c>
       <c r="C12" s="10">
         <f t="shared" si="0"/>
-        <v>4666.666666666667</v>
+        <v>2616.2999999999997</v>
       </c>
       <c r="D12" s="10">
         <f t="shared" si="0"/>
-        <v>4200</v>
+        <v>2325.6</v>
       </c>
       <c r="E12" s="10">
         <f t="shared" si="0"/>
-        <v>3818.181818181818</v>
-      </c>
-      <c r="F12" s="11">
-        <f t="shared" si="0"/>
-        <v>3500</v>
+        <v>2093.0399999999995</v>
+      </c>
+      <c r="F12" s="10">
+        <f t="shared" si="0"/>
+        <v>1902.7636363636364</v>
+      </c>
+      <c r="G12" s="11">
+        <f t="shared" si="0"/>
+        <v>1744.1999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="32.25" customHeight="1">
+    <row r="13" spans="1:253" ht="32.25" customHeight="1">
       <c r="A13" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="10">
         <f t="shared" si="1"/>
-        <v>5333.3333333333339</v>
+        <v>3052.35</v>
       </c>
       <c r="C13" s="10">
         <f t="shared" si="0"/>
-        <v>4800</v>
+        <v>2713.2</v>
       </c>
       <c r="D13" s="10">
         <f t="shared" si="0"/>
-        <v>4363.636363636364</v>
+        <v>2441.8799999999997</v>
       </c>
       <c r="E13" s="10">
         <f t="shared" si="0"/>
-        <v>4000</v>
-      </c>
-      <c r="F13" s="11">
-        <f t="shared" si="0"/>
-        <v>3692.3076923076924</v>
+        <v>2219.8909090909087</v>
+      </c>
+      <c r="F13" s="10">
+        <f t="shared" si="0"/>
+        <v>2034.8999999999999</v>
+      </c>
+      <c r="G13" s="11">
+        <f t="shared" si="0"/>
+        <v>1878.3692307692306</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="32.25" customHeight="1">
+    <row r="14" spans="1:253" ht="32.25" customHeight="1">
       <c r="A14" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="10">
         <f t="shared" si="1"/>
-        <v>5400</v>
+        <v>3100.7999999999997</v>
       </c>
       <c r="C14" s="10">
         <f t="shared" si="0"/>
-        <v>4909.090909090909</v>
+        <v>2790.7200000000003</v>
       </c>
       <c r="D14" s="10">
         <f t="shared" si="0"/>
-        <v>4500</v>
+        <v>2537.0181818181818</v>
       </c>
       <c r="E14" s="10">
         <f t="shared" si="0"/>
-        <v>4153.8461538461534</v>
-      </c>
-      <c r="F14" s="11">
-        <f t="shared" si="0"/>
-        <v>3857.1428571428573</v>
+        <v>2325.6</v>
+      </c>
+      <c r="F14" s="10">
+        <f t="shared" si="0"/>
+        <v>2146.707692307692</v>
+      </c>
+      <c r="G14" s="11">
+        <f t="shared" si="0"/>
+        <v>1993.3714285714284</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="32.25" customHeight="1">
+    <row r="15" spans="1:253" ht="32.25" customHeight="1">
       <c r="A15" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="10">
         <f t="shared" si="1"/>
-        <v>5454.545454545455</v>
+        <v>3139.5599999999995</v>
       </c>
       <c r="C15" s="10">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>2854.1454545454544</v>
       </c>
       <c r="D15" s="10">
         <f t="shared" si="0"/>
-        <v>4615.3846153846152</v>
+        <v>2616.2999999999997</v>
       </c>
       <c r="E15" s="10">
         <f t="shared" si="0"/>
-        <v>4285.7142857142862</v>
-      </c>
-      <c r="F15" s="11">
-        <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>2415.0461538461536</v>
+      </c>
+      <c r="F15" s="10">
+        <f t="shared" si="0"/>
+        <v>2242.542857142857</v>
+      </c>
+      <c r="G15" s="11">
+        <f t="shared" si="0"/>
+        <v>2093.0399999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" customHeight="1">
-      <c r="A17" s="18" t="s">
+    <row r="16" spans="1:253" ht="32.25" customHeight="1">
+      <c r="A16" s="3">
+        <v>10</v>
+      </c>
+      <c r="B16" s="10">
+        <f t="shared" si="1"/>
+        <v>3171.272727272727</v>
+      </c>
+      <c r="C16" s="10">
+        <f t="shared" si="0"/>
+        <v>2907</v>
+      </c>
+      <c r="D16" s="10">
+        <f t="shared" si="0"/>
+        <v>2683.3846153846152</v>
+      </c>
+      <c r="E16" s="10">
+        <f t="shared" si="0"/>
+        <v>2491.7142857142858</v>
+      </c>
+      <c r="F16" s="10">
+        <f t="shared" si="0"/>
+        <v>2325.6</v>
+      </c>
+      <c r="G16" s="11">
+        <f t="shared" si="0"/>
+        <v>2180.25</v>
+      </c>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="17"/>
+      <c r="Z16" s="17"/>
+      <c r="AA16" s="17"/>
+      <c r="AB16" s="17"/>
+      <c r="AC16" s="17"/>
+      <c r="AD16" s="17"/>
+      <c r="AE16" s="17"/>
+      <c r="AF16" s="17"/>
+      <c r="AG16" s="17"/>
+      <c r="AH16" s="17"/>
+      <c r="AI16" s="17"/>
+      <c r="AJ16" s="17"/>
+      <c r="AK16" s="17"/>
+      <c r="AL16" s="17"/>
+      <c r="AM16" s="17"/>
+      <c r="AN16" s="17"/>
+      <c r="AO16" s="17"/>
+      <c r="AP16" s="17"/>
+      <c r="AQ16" s="17"/>
+      <c r="AR16" s="17"/>
+      <c r="AS16" s="17"/>
+      <c r="AT16" s="17"/>
+      <c r="AU16" s="17"/>
+      <c r="AV16" s="17"/>
+      <c r="AW16" s="17"/>
+      <c r="AX16" s="17"/>
+      <c r="AY16" s="17"/>
+      <c r="AZ16" s="17"/>
+      <c r="BA16" s="17"/>
+      <c r="BB16" s="17"/>
+      <c r="BC16" s="17"/>
+      <c r="BD16" s="17"/>
+      <c r="BE16" s="17"/>
+      <c r="BF16" s="17"/>
+      <c r="BG16" s="17"/>
+      <c r="BH16" s="17"/>
+      <c r="BI16" s="17"/>
+      <c r="BJ16" s="17"/>
+      <c r="BK16" s="17"/>
+      <c r="BL16" s="17"/>
+      <c r="BM16" s="17"/>
+      <c r="BN16" s="17"/>
+      <c r="BO16" s="17"/>
+      <c r="BP16" s="17"/>
+      <c r="BQ16" s="17"/>
+      <c r="BR16" s="17"/>
+      <c r="BS16" s="17"/>
+      <c r="BT16" s="17"/>
+      <c r="BU16" s="17"/>
+      <c r="BV16" s="17"/>
+      <c r="BW16" s="17"/>
+      <c r="BX16" s="17"/>
+      <c r="BY16" s="17"/>
+      <c r="BZ16" s="17"/>
+      <c r="CA16" s="17"/>
+      <c r="CB16" s="17"/>
+      <c r="CC16" s="17"/>
+      <c r="CD16" s="17"/>
+      <c r="CE16" s="17"/>
+      <c r="CF16" s="17"/>
+      <c r="CG16" s="17"/>
+      <c r="CH16" s="17"/>
+      <c r="CI16" s="17"/>
+      <c r="CJ16" s="17"/>
+      <c r="CK16" s="17"/>
+      <c r="CL16" s="17"/>
+      <c r="CM16" s="17"/>
+      <c r="CN16" s="17"/>
+      <c r="CO16" s="17"/>
+      <c r="CP16" s="17"/>
+      <c r="CQ16" s="17"/>
+      <c r="CR16" s="17"/>
+      <c r="CS16" s="17"/>
+      <c r="CT16" s="17"/>
+      <c r="CU16" s="17"/>
+      <c r="CV16" s="17"/>
+      <c r="CW16" s="17"/>
+      <c r="CX16" s="17"/>
+      <c r="CY16" s="17"/>
+      <c r="CZ16" s="17"/>
+      <c r="DA16" s="17"/>
+      <c r="DB16" s="17"/>
+      <c r="DC16" s="17"/>
+      <c r="DD16" s="17"/>
+      <c r="DE16" s="17"/>
+      <c r="DF16" s="17"/>
+      <c r="DG16" s="17"/>
+      <c r="DH16" s="17"/>
+      <c r="DI16" s="17"/>
+      <c r="DJ16" s="17"/>
+      <c r="DK16" s="17"/>
+      <c r="DL16" s="17"/>
+      <c r="DM16" s="17"/>
+      <c r="DN16" s="17"/>
+      <c r="DO16" s="17"/>
+      <c r="DP16" s="17"/>
+      <c r="DQ16" s="17"/>
+      <c r="DR16" s="17"/>
+      <c r="DS16" s="17"/>
+      <c r="DT16" s="17"/>
+      <c r="DU16" s="17"/>
+      <c r="DV16" s="17"/>
+      <c r="DW16" s="17"/>
+      <c r="DX16" s="17"/>
+      <c r="DY16" s="17"/>
+      <c r="DZ16" s="17"/>
+      <c r="EA16" s="17"/>
+      <c r="EB16" s="17"/>
+      <c r="EC16" s="17"/>
+      <c r="ED16" s="17"/>
+      <c r="EE16" s="17"/>
+      <c r="EF16" s="17"/>
+      <c r="EG16" s="17"/>
+      <c r="EH16" s="17"/>
+      <c r="EI16" s="17"/>
+      <c r="EJ16" s="17"/>
+      <c r="EK16" s="17"/>
+      <c r="EL16" s="17"/>
+      <c r="EM16" s="17"/>
+      <c r="EN16" s="17"/>
+      <c r="EO16" s="17"/>
+      <c r="EP16" s="17"/>
+      <c r="EQ16" s="17"/>
+      <c r="ER16" s="17"/>
+      <c r="ES16" s="17"/>
+      <c r="ET16" s="17"/>
+      <c r="EU16" s="17"/>
+      <c r="EV16" s="17"/>
+      <c r="EW16" s="17"/>
+      <c r="EX16" s="17"/>
+      <c r="EY16" s="17"/>
+      <c r="EZ16" s="17"/>
+      <c r="FA16" s="17"/>
+      <c r="FB16" s="17"/>
+      <c r="FC16" s="17"/>
+      <c r="FD16" s="17"/>
+      <c r="FE16" s="17"/>
+      <c r="FF16" s="17"/>
+      <c r="FG16" s="17"/>
+      <c r="FH16" s="17"/>
+      <c r="FI16" s="17"/>
+      <c r="FJ16" s="17"/>
+      <c r="FK16" s="17"/>
+      <c r="FL16" s="17"/>
+      <c r="FM16" s="17"/>
+      <c r="FN16" s="17"/>
+      <c r="FO16" s="17"/>
+      <c r="FP16" s="17"/>
+      <c r="FQ16" s="17"/>
+      <c r="FR16" s="17"/>
+      <c r="FS16" s="17"/>
+      <c r="FT16" s="17"/>
+      <c r="FU16" s="17"/>
+      <c r="FV16" s="17"/>
+      <c r="FW16" s="17"/>
+      <c r="FX16" s="17"/>
+      <c r="FY16" s="17"/>
+      <c r="FZ16" s="17"/>
+      <c r="GA16" s="17"/>
+      <c r="GB16" s="17"/>
+      <c r="GC16" s="17"/>
+      <c r="GD16" s="17"/>
+      <c r="GE16" s="17"/>
+      <c r="GF16" s="17"/>
+      <c r="GG16" s="17"/>
+      <c r="GH16" s="17"/>
+      <c r="GI16" s="17"/>
+      <c r="GJ16" s="17"/>
+      <c r="GK16" s="17"/>
+      <c r="GL16" s="17"/>
+      <c r="GM16" s="17"/>
+      <c r="GN16" s="17"/>
+      <c r="GO16" s="17"/>
+      <c r="GP16" s="17"/>
+      <c r="GQ16" s="17"/>
+      <c r="GR16" s="17"/>
+      <c r="GS16" s="17"/>
+      <c r="GT16" s="17"/>
+      <c r="GU16" s="17"/>
+      <c r="GV16" s="17"/>
+      <c r="GW16" s="17"/>
+      <c r="GX16" s="17"/>
+      <c r="GY16" s="17"/>
+      <c r="GZ16" s="17"/>
+      <c r="HA16" s="17"/>
+      <c r="HB16" s="17"/>
+      <c r="HC16" s="17"/>
+      <c r="HD16" s="17"/>
+      <c r="HE16" s="17"/>
+      <c r="HF16" s="17"/>
+      <c r="HG16" s="17"/>
+      <c r="HH16" s="17"/>
+      <c r="HI16" s="17"/>
+      <c r="HJ16" s="17"/>
+      <c r="HK16" s="17"/>
+      <c r="HL16" s="17"/>
+      <c r="HM16" s="17"/>
+      <c r="HN16" s="17"/>
+      <c r="HO16" s="17"/>
+      <c r="HP16" s="17"/>
+      <c r="HQ16" s="17"/>
+      <c r="HR16" s="17"/>
+      <c r="HS16" s="17"/>
+      <c r="HT16" s="17"/>
+      <c r="HU16" s="17"/>
+      <c r="HV16" s="17"/>
+      <c r="HW16" s="17"/>
+      <c r="HX16" s="17"/>
+      <c r="HY16" s="17"/>
+      <c r="HZ16" s="17"/>
+      <c r="IA16" s="17"/>
+      <c r="IB16" s="17"/>
+      <c r="IC16" s="17"/>
+      <c r="ID16" s="17"/>
+      <c r="IE16" s="17"/>
+      <c r="IF16" s="17"/>
+      <c r="IG16" s="17"/>
+      <c r="IH16" s="17"/>
+      <c r="II16" s="17"/>
+      <c r="IJ16" s="17"/>
+      <c r="IK16" s="17"/>
+      <c r="IL16" s="17"/>
+      <c r="IM16" s="17"/>
+      <c r="IN16" s="17"/>
+      <c r="IO16" s="17"/>
+      <c r="IP16" s="17"/>
+      <c r="IQ16" s="17"/>
+      <c r="IR16" s="17"/>
+      <c r="IS16" s="17"/>
+    </row>
+    <row r="17" spans="1:253" ht="32.25" customHeight="1">
+      <c r="A17" s="3">
+        <v>11</v>
+      </c>
+      <c r="B17" s="10">
+        <f t="shared" si="1"/>
+        <v>3197.7</v>
+      </c>
+      <c r="C17" s="10">
+        <f t="shared" si="0"/>
+        <v>2951.7230769230764</v>
+      </c>
+      <c r="D17" s="10">
+        <f t="shared" si="0"/>
+        <v>2740.8857142857141</v>
+      </c>
+      <c r="E17" s="10">
+        <f t="shared" si="0"/>
+        <v>2558.16</v>
+      </c>
+      <c r="F17" s="10">
+        <f t="shared" si="0"/>
+        <v>2398.2750000000001</v>
+      </c>
+      <c r="G17" s="11">
+        <f t="shared" si="0"/>
+        <v>2257.1999999999998</v>
+      </c>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="17"/>
+      <c r="V17" s="17"/>
+      <c r="W17" s="17"/>
+      <c r="X17" s="17"/>
+      <c r="Y17" s="17"/>
+      <c r="Z17" s="17"/>
+      <c r="AA17" s="17"/>
+      <c r="AB17" s="17"/>
+      <c r="AC17" s="17"/>
+      <c r="AD17" s="17"/>
+      <c r="AE17" s="17"/>
+      <c r="AF17" s="17"/>
+      <c r="AG17" s="17"/>
+      <c r="AH17" s="17"/>
+      <c r="AI17" s="17"/>
+      <c r="AJ17" s="17"/>
+      <c r="AK17" s="17"/>
+      <c r="AL17" s="17"/>
+      <c r="AM17" s="17"/>
+      <c r="AN17" s="17"/>
+      <c r="AO17" s="17"/>
+      <c r="AP17" s="17"/>
+      <c r="AQ17" s="17"/>
+      <c r="AR17" s="17"/>
+      <c r="AS17" s="17"/>
+      <c r="AT17" s="17"/>
+      <c r="AU17" s="17"/>
+      <c r="AV17" s="17"/>
+      <c r="AW17" s="17"/>
+      <c r="AX17" s="17"/>
+      <c r="AY17" s="17"/>
+      <c r="AZ17" s="17"/>
+      <c r="BA17" s="17"/>
+      <c r="BB17" s="17"/>
+      <c r="BC17" s="17"/>
+      <c r="BD17" s="17"/>
+      <c r="BE17" s="17"/>
+      <c r="BF17" s="17"/>
+      <c r="BG17" s="17"/>
+      <c r="BH17" s="17"/>
+      <c r="BI17" s="17"/>
+      <c r="BJ17" s="17"/>
+      <c r="BK17" s="17"/>
+      <c r="BL17" s="17"/>
+      <c r="BM17" s="17"/>
+      <c r="BN17" s="17"/>
+      <c r="BO17" s="17"/>
+      <c r="BP17" s="17"/>
+      <c r="BQ17" s="17"/>
+      <c r="BR17" s="17"/>
+      <c r="BS17" s="17"/>
+      <c r="BT17" s="17"/>
+      <c r="BU17" s="17"/>
+      <c r="BV17" s="17"/>
+      <c r="BW17" s="17"/>
+      <c r="BX17" s="17"/>
+      <c r="BY17" s="17"/>
+      <c r="BZ17" s="17"/>
+      <c r="CA17" s="17"/>
+      <c r="CB17" s="17"/>
+      <c r="CC17" s="17"/>
+      <c r="CD17" s="17"/>
+      <c r="CE17" s="17"/>
+      <c r="CF17" s="17"/>
+      <c r="CG17" s="17"/>
+      <c r="CH17" s="17"/>
+      <c r="CI17" s="17"/>
+      <c r="CJ17" s="17"/>
+      <c r="CK17" s="17"/>
+      <c r="CL17" s="17"/>
+      <c r="CM17" s="17"/>
+      <c r="CN17" s="17"/>
+      <c r="CO17" s="17"/>
+      <c r="CP17" s="17"/>
+      <c r="CQ17" s="17"/>
+      <c r="CR17" s="17"/>
+      <c r="CS17" s="17"/>
+      <c r="CT17" s="17"/>
+      <c r="CU17" s="17"/>
+      <c r="CV17" s="17"/>
+      <c r="CW17" s="17"/>
+      <c r="CX17" s="17"/>
+      <c r="CY17" s="17"/>
+      <c r="CZ17" s="17"/>
+      <c r="DA17" s="17"/>
+      <c r="DB17" s="17"/>
+      <c r="DC17" s="17"/>
+      <c r="DD17" s="17"/>
+      <c r="DE17" s="17"/>
+      <c r="DF17" s="17"/>
+      <c r="DG17" s="17"/>
+      <c r="DH17" s="17"/>
+      <c r="DI17" s="17"/>
+      <c r="DJ17" s="17"/>
+      <c r="DK17" s="17"/>
+      <c r="DL17" s="17"/>
+      <c r="DM17" s="17"/>
+      <c r="DN17" s="17"/>
+      <c r="DO17" s="17"/>
+      <c r="DP17" s="17"/>
+      <c r="DQ17" s="17"/>
+      <c r="DR17" s="17"/>
+      <c r="DS17" s="17"/>
+      <c r="DT17" s="17"/>
+      <c r="DU17" s="17"/>
+      <c r="DV17" s="17"/>
+      <c r="DW17" s="17"/>
+      <c r="DX17" s="17"/>
+      <c r="DY17" s="17"/>
+      <c r="DZ17" s="17"/>
+      <c r="EA17" s="17"/>
+      <c r="EB17" s="17"/>
+      <c r="EC17" s="17"/>
+      <c r="ED17" s="17"/>
+      <c r="EE17" s="17"/>
+      <c r="EF17" s="17"/>
+      <c r="EG17" s="17"/>
+      <c r="EH17" s="17"/>
+      <c r="EI17" s="17"/>
+      <c r="EJ17" s="17"/>
+      <c r="EK17" s="17"/>
+      <c r="EL17" s="17"/>
+      <c r="EM17" s="17"/>
+      <c r="EN17" s="17"/>
+      <c r="EO17" s="17"/>
+      <c r="EP17" s="17"/>
+      <c r="EQ17" s="17"/>
+      <c r="ER17" s="17"/>
+      <c r="ES17" s="17"/>
+      <c r="ET17" s="17"/>
+      <c r="EU17" s="17"/>
+      <c r="EV17" s="17"/>
+      <c r="EW17" s="17"/>
+      <c r="EX17" s="17"/>
+      <c r="EY17" s="17"/>
+      <c r="EZ17" s="17"/>
+      <c r="FA17" s="17"/>
+      <c r="FB17" s="17"/>
+      <c r="FC17" s="17"/>
+      <c r="FD17" s="17"/>
+      <c r="FE17" s="17"/>
+      <c r="FF17" s="17"/>
+      <c r="FG17" s="17"/>
+      <c r="FH17" s="17"/>
+      <c r="FI17" s="17"/>
+      <c r="FJ17" s="17"/>
+      <c r="FK17" s="17"/>
+      <c r="FL17" s="17"/>
+      <c r="FM17" s="17"/>
+      <c r="FN17" s="17"/>
+      <c r="FO17" s="17"/>
+      <c r="FP17" s="17"/>
+      <c r="FQ17" s="17"/>
+      <c r="FR17" s="17"/>
+      <c r="FS17" s="17"/>
+      <c r="FT17" s="17"/>
+      <c r="FU17" s="17"/>
+      <c r="FV17" s="17"/>
+      <c r="FW17" s="17"/>
+      <c r="FX17" s="17"/>
+      <c r="FY17" s="17"/>
+      <c r="FZ17" s="17"/>
+      <c r="GA17" s="17"/>
+      <c r="GB17" s="17"/>
+      <c r="GC17" s="17"/>
+      <c r="GD17" s="17"/>
+      <c r="GE17" s="17"/>
+      <c r="GF17" s="17"/>
+      <c r="GG17" s="17"/>
+      <c r="GH17" s="17"/>
+      <c r="GI17" s="17"/>
+      <c r="GJ17" s="17"/>
+      <c r="GK17" s="17"/>
+      <c r="GL17" s="17"/>
+      <c r="GM17" s="17"/>
+      <c r="GN17" s="17"/>
+      <c r="GO17" s="17"/>
+      <c r="GP17" s="17"/>
+      <c r="GQ17" s="17"/>
+      <c r="GR17" s="17"/>
+      <c r="GS17" s="17"/>
+      <c r="GT17" s="17"/>
+      <c r="GU17" s="17"/>
+      <c r="GV17" s="17"/>
+      <c r="GW17" s="17"/>
+      <c r="GX17" s="17"/>
+      <c r="GY17" s="17"/>
+      <c r="GZ17" s="17"/>
+      <c r="HA17" s="17"/>
+      <c r="HB17" s="17"/>
+      <c r="HC17" s="17"/>
+      <c r="HD17" s="17"/>
+      <c r="HE17" s="17"/>
+      <c r="HF17" s="17"/>
+      <c r="HG17" s="17"/>
+      <c r="HH17" s="17"/>
+      <c r="HI17" s="17"/>
+      <c r="HJ17" s="17"/>
+      <c r="HK17" s="17"/>
+      <c r="HL17" s="17"/>
+      <c r="HM17" s="17"/>
+      <c r="HN17" s="17"/>
+      <c r="HO17" s="17"/>
+      <c r="HP17" s="17"/>
+      <c r="HQ17" s="17"/>
+      <c r="HR17" s="17"/>
+      <c r="HS17" s="17"/>
+      <c r="HT17" s="17"/>
+      <c r="HU17" s="17"/>
+      <c r="HV17" s="17"/>
+      <c r="HW17" s="17"/>
+      <c r="HX17" s="17"/>
+      <c r="HY17" s="17"/>
+      <c r="HZ17" s="17"/>
+      <c r="IA17" s="17"/>
+      <c r="IB17" s="17"/>
+      <c r="IC17" s="17"/>
+      <c r="ID17" s="17"/>
+      <c r="IE17" s="17"/>
+      <c r="IF17" s="17"/>
+      <c r="IG17" s="17"/>
+      <c r="IH17" s="17"/>
+      <c r="II17" s="17"/>
+      <c r="IJ17" s="17"/>
+      <c r="IK17" s="17"/>
+      <c r="IL17" s="17"/>
+      <c r="IM17" s="17"/>
+      <c r="IN17" s="17"/>
+      <c r="IO17" s="17"/>
+      <c r="IP17" s="17"/>
+      <c r="IQ17" s="17"/>
+      <c r="IR17" s="17"/>
+      <c r="IS17" s="17"/>
+    </row>
+    <row r="18" spans="1:253" ht="32.25" customHeight="1">
+      <c r="A18" s="3">
+        <v>12</v>
+      </c>
+      <c r="B18" s="10">
+        <f t="shared" si="1"/>
+        <v>3220.061538461538</v>
+      </c>
+      <c r="C18" s="10">
+        <f t="shared" si="0"/>
+        <v>2990.0571428571429</v>
+      </c>
+      <c r="D18" s="10">
+        <f t="shared" si="0"/>
+        <v>2790.7200000000003</v>
+      </c>
+      <c r="E18" s="10">
+        <f t="shared" si="0"/>
+        <v>2616.2999999999997</v>
+      </c>
+      <c r="F18" s="10">
+        <f t="shared" si="0"/>
+        <v>2462.4</v>
+      </c>
+      <c r="G18" s="11">
+        <f t="shared" si="0"/>
+        <v>2325.6</v>
+      </c>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="17"/>
+      <c r="W18" s="17"/>
+      <c r="X18" s="17"/>
+      <c r="Y18" s="17"/>
+      <c r="Z18" s="17"/>
+      <c r="AA18" s="17"/>
+      <c r="AB18" s="17"/>
+      <c r="AC18" s="17"/>
+      <c r="AD18" s="17"/>
+      <c r="AE18" s="17"/>
+      <c r="AF18" s="17"/>
+      <c r="AG18" s="17"/>
+      <c r="AH18" s="17"/>
+      <c r="AI18" s="17"/>
+      <c r="AJ18" s="17"/>
+      <c r="AK18" s="17"/>
+      <c r="AL18" s="17"/>
+      <c r="AM18" s="17"/>
+      <c r="AN18" s="17"/>
+      <c r="AO18" s="17"/>
+      <c r="AP18" s="17"/>
+      <c r="AQ18" s="17"/>
+      <c r="AR18" s="17"/>
+      <c r="AS18" s="17"/>
+      <c r="AT18" s="17"/>
+      <c r="AU18" s="17"/>
+      <c r="AV18" s="17"/>
+      <c r="AW18" s="17"/>
+      <c r="AX18" s="17"/>
+      <c r="AY18" s="17"/>
+      <c r="AZ18" s="17"/>
+      <c r="BA18" s="17"/>
+      <c r="BB18" s="17"/>
+      <c r="BC18" s="17"/>
+      <c r="BD18" s="17"/>
+      <c r="BE18" s="17"/>
+      <c r="BF18" s="17"/>
+      <c r="BG18" s="17"/>
+      <c r="BH18" s="17"/>
+      <c r="BI18" s="17"/>
+      <c r="BJ18" s="17"/>
+      <c r="BK18" s="17"/>
+      <c r="BL18" s="17"/>
+      <c r="BM18" s="17"/>
+      <c r="BN18" s="17"/>
+      <c r="BO18" s="17"/>
+      <c r="BP18" s="17"/>
+      <c r="BQ18" s="17"/>
+      <c r="BR18" s="17"/>
+      <c r="BS18" s="17"/>
+      <c r="BT18" s="17"/>
+      <c r="BU18" s="17"/>
+      <c r="BV18" s="17"/>
+      <c r="BW18" s="17"/>
+      <c r="BX18" s="17"/>
+      <c r="BY18" s="17"/>
+      <c r="BZ18" s="17"/>
+      <c r="CA18" s="17"/>
+      <c r="CB18" s="17"/>
+      <c r="CC18" s="17"/>
+      <c r="CD18" s="17"/>
+      <c r="CE18" s="17"/>
+      <c r="CF18" s="17"/>
+      <c r="CG18" s="17"/>
+      <c r="CH18" s="17"/>
+      <c r="CI18" s="17"/>
+      <c r="CJ18" s="17"/>
+      <c r="CK18" s="17"/>
+      <c r="CL18" s="17"/>
+      <c r="CM18" s="17"/>
+      <c r="CN18" s="17"/>
+      <c r="CO18" s="17"/>
+      <c r="CP18" s="17"/>
+      <c r="CQ18" s="17"/>
+      <c r="CR18" s="17"/>
+      <c r="CS18" s="17"/>
+      <c r="CT18" s="17"/>
+      <c r="CU18" s="17"/>
+      <c r="CV18" s="17"/>
+      <c r="CW18" s="17"/>
+      <c r="CX18" s="17"/>
+      <c r="CY18" s="17"/>
+      <c r="CZ18" s="17"/>
+      <c r="DA18" s="17"/>
+      <c r="DB18" s="17"/>
+      <c r="DC18" s="17"/>
+      <c r="DD18" s="17"/>
+      <c r="DE18" s="17"/>
+      <c r="DF18" s="17"/>
+      <c r="DG18" s="17"/>
+      <c r="DH18" s="17"/>
+      <c r="DI18" s="17"/>
+      <c r="DJ18" s="17"/>
+      <c r="DK18" s="17"/>
+      <c r="DL18" s="17"/>
+      <c r="DM18" s="17"/>
+      <c r="DN18" s="17"/>
+      <c r="DO18" s="17"/>
+      <c r="DP18" s="17"/>
+      <c r="DQ18" s="17"/>
+      <c r="DR18" s="17"/>
+      <c r="DS18" s="17"/>
+      <c r="DT18" s="17"/>
+      <c r="DU18" s="17"/>
+      <c r="DV18" s="17"/>
+      <c r="DW18" s="17"/>
+      <c r="DX18" s="17"/>
+      <c r="DY18" s="17"/>
+      <c r="DZ18" s="17"/>
+      <c r="EA18" s="17"/>
+      <c r="EB18" s="17"/>
+      <c r="EC18" s="17"/>
+      <c r="ED18" s="17"/>
+      <c r="EE18" s="17"/>
+      <c r="EF18" s="17"/>
+      <c r="EG18" s="17"/>
+      <c r="EH18" s="17"/>
+      <c r="EI18" s="17"/>
+      <c r="EJ18" s="17"/>
+      <c r="EK18" s="17"/>
+      <c r="EL18" s="17"/>
+      <c r="EM18" s="17"/>
+      <c r="EN18" s="17"/>
+      <c r="EO18" s="17"/>
+      <c r="EP18" s="17"/>
+      <c r="EQ18" s="17"/>
+      <c r="ER18" s="17"/>
+      <c r="ES18" s="17"/>
+      <c r="ET18" s="17"/>
+      <c r="EU18" s="17"/>
+      <c r="EV18" s="17"/>
+      <c r="EW18" s="17"/>
+      <c r="EX18" s="17"/>
+      <c r="EY18" s="17"/>
+      <c r="EZ18" s="17"/>
+      <c r="FA18" s="17"/>
+      <c r="FB18" s="17"/>
+      <c r="FC18" s="17"/>
+      <c r="FD18" s="17"/>
+      <c r="FE18" s="17"/>
+      <c r="FF18" s="17"/>
+      <c r="FG18" s="17"/>
+      <c r="FH18" s="17"/>
+      <c r="FI18" s="17"/>
+      <c r="FJ18" s="17"/>
+      <c r="FK18" s="17"/>
+      <c r="FL18" s="17"/>
+      <c r="FM18" s="17"/>
+      <c r="FN18" s="17"/>
+      <c r="FO18" s="17"/>
+      <c r="FP18" s="17"/>
+      <c r="FQ18" s="17"/>
+      <c r="FR18" s="17"/>
+      <c r="FS18" s="17"/>
+      <c r="FT18" s="17"/>
+      <c r="FU18" s="17"/>
+      <c r="FV18" s="17"/>
+      <c r="FW18" s="17"/>
+      <c r="FX18" s="17"/>
+      <c r="FY18" s="17"/>
+      <c r="FZ18" s="17"/>
+      <c r="GA18" s="17"/>
+      <c r="GB18" s="17"/>
+      <c r="GC18" s="17"/>
+      <c r="GD18" s="17"/>
+      <c r="GE18" s="17"/>
+      <c r="GF18" s="17"/>
+      <c r="GG18" s="17"/>
+      <c r="GH18" s="17"/>
+      <c r="GI18" s="17"/>
+      <c r="GJ18" s="17"/>
+      <c r="GK18" s="17"/>
+      <c r="GL18" s="17"/>
+      <c r="GM18" s="17"/>
+      <c r="GN18" s="17"/>
+      <c r="GO18" s="17"/>
+      <c r="GP18" s="17"/>
+      <c r="GQ18" s="17"/>
+      <c r="GR18" s="17"/>
+      <c r="GS18" s="17"/>
+      <c r="GT18" s="17"/>
+      <c r="GU18" s="17"/>
+      <c r="GV18" s="17"/>
+      <c r="GW18" s="17"/>
+      <c r="GX18" s="17"/>
+      <c r="GY18" s="17"/>
+      <c r="GZ18" s="17"/>
+      <c r="HA18" s="17"/>
+      <c r="HB18" s="17"/>
+      <c r="HC18" s="17"/>
+      <c r="HD18" s="17"/>
+      <c r="HE18" s="17"/>
+      <c r="HF18" s="17"/>
+      <c r="HG18" s="17"/>
+      <c r="HH18" s="17"/>
+      <c r="HI18" s="17"/>
+      <c r="HJ18" s="17"/>
+      <c r="HK18" s="17"/>
+      <c r="HL18" s="17"/>
+      <c r="HM18" s="17"/>
+      <c r="HN18" s="17"/>
+      <c r="HO18" s="17"/>
+      <c r="HP18" s="17"/>
+      <c r="HQ18" s="17"/>
+      <c r="HR18" s="17"/>
+      <c r="HS18" s="17"/>
+      <c r="HT18" s="17"/>
+      <c r="HU18" s="17"/>
+      <c r="HV18" s="17"/>
+      <c r="HW18" s="17"/>
+      <c r="HX18" s="17"/>
+      <c r="HY18" s="17"/>
+      <c r="HZ18" s="17"/>
+      <c r="IA18" s="17"/>
+      <c r="IB18" s="17"/>
+      <c r="IC18" s="17"/>
+      <c r="ID18" s="17"/>
+      <c r="IE18" s="17"/>
+      <c r="IF18" s="17"/>
+      <c r="IG18" s="17"/>
+      <c r="IH18" s="17"/>
+      <c r="II18" s="17"/>
+      <c r="IJ18" s="17"/>
+      <c r="IK18" s="17"/>
+      <c r="IL18" s="17"/>
+      <c r="IM18" s="17"/>
+      <c r="IN18" s="17"/>
+      <c r="IO18" s="17"/>
+      <c r="IP18" s="17"/>
+      <c r="IQ18" s="17"/>
+      <c r="IR18" s="17"/>
+      <c r="IS18" s="17"/>
+    </row>
+    <row r="19" spans="1:253" ht="32.25" customHeight="1">
+      <c r="A19" s="3">
+        <v>13</v>
+      </c>
+      <c r="B19" s="10">
+        <f t="shared" si="1"/>
+        <v>3239.2285714285717</v>
+      </c>
+      <c r="C19" s="10">
+        <f t="shared" si="0"/>
+        <v>3023.2799999999993</v>
+      </c>
+      <c r="D19" s="10">
+        <f t="shared" si="0"/>
+        <v>2834.3249999999998</v>
+      </c>
+      <c r="E19" s="10">
+        <f t="shared" si="0"/>
+        <v>2667.6</v>
+      </c>
+      <c r="F19" s="10">
+        <f t="shared" si="0"/>
+        <v>2519.4</v>
+      </c>
+      <c r="G19" s="11">
+        <f t="shared" si="0"/>
+        <v>2386.8000000000002</v>
+      </c>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="17"/>
+      <c r="Y19" s="17"/>
+      <c r="Z19" s="17"/>
+      <c r="AA19" s="17"/>
+      <c r="AB19" s="17"/>
+      <c r="AC19" s="17"/>
+      <c r="AD19" s="17"/>
+      <c r="AE19" s="17"/>
+      <c r="AF19" s="17"/>
+      <c r="AG19" s="17"/>
+      <c r="AH19" s="17"/>
+      <c r="AI19" s="17"/>
+      <c r="AJ19" s="17"/>
+      <c r="AK19" s="17"/>
+      <c r="AL19" s="17"/>
+      <c r="AM19" s="17"/>
+      <c r="AN19" s="17"/>
+      <c r="AO19" s="17"/>
+      <c r="AP19" s="17"/>
+      <c r="AQ19" s="17"/>
+      <c r="AR19" s="17"/>
+      <c r="AS19" s="17"/>
+      <c r="AT19" s="17"/>
+      <c r="AU19" s="17"/>
+      <c r="AV19" s="17"/>
+      <c r="AW19" s="17"/>
+      <c r="AX19" s="17"/>
+      <c r="AY19" s="17"/>
+      <c r="AZ19" s="17"/>
+      <c r="BA19" s="17"/>
+      <c r="BB19" s="17"/>
+      <c r="BC19" s="17"/>
+      <c r="BD19" s="17"/>
+      <c r="BE19" s="17"/>
+      <c r="BF19" s="17"/>
+      <c r="BG19" s="17"/>
+      <c r="BH19" s="17"/>
+      <c r="BI19" s="17"/>
+      <c r="BJ19" s="17"/>
+      <c r="BK19" s="17"/>
+      <c r="BL19" s="17"/>
+      <c r="BM19" s="17"/>
+      <c r="BN19" s="17"/>
+      <c r="BO19" s="17"/>
+      <c r="BP19" s="17"/>
+      <c r="BQ19" s="17"/>
+      <c r="BR19" s="17"/>
+      <c r="BS19" s="17"/>
+      <c r="BT19" s="17"/>
+      <c r="BU19" s="17"/>
+      <c r="BV19" s="17"/>
+      <c r="BW19" s="17"/>
+      <c r="BX19" s="17"/>
+      <c r="BY19" s="17"/>
+      <c r="BZ19" s="17"/>
+      <c r="CA19" s="17"/>
+      <c r="CB19" s="17"/>
+      <c r="CC19" s="17"/>
+      <c r="CD19" s="17"/>
+      <c r="CE19" s="17"/>
+      <c r="CF19" s="17"/>
+      <c r="CG19" s="17"/>
+      <c r="CH19" s="17"/>
+      <c r="CI19" s="17"/>
+      <c r="CJ19" s="17"/>
+      <c r="CK19" s="17"/>
+      <c r="CL19" s="17"/>
+      <c r="CM19" s="17"/>
+      <c r="CN19" s="17"/>
+      <c r="CO19" s="17"/>
+      <c r="CP19" s="17"/>
+      <c r="CQ19" s="17"/>
+      <c r="CR19" s="17"/>
+      <c r="CS19" s="17"/>
+      <c r="CT19" s="17"/>
+      <c r="CU19" s="17"/>
+      <c r="CV19" s="17"/>
+      <c r="CW19" s="17"/>
+      <c r="CX19" s="17"/>
+      <c r="CY19" s="17"/>
+      <c r="CZ19" s="17"/>
+      <c r="DA19" s="17"/>
+      <c r="DB19" s="17"/>
+      <c r="DC19" s="17"/>
+      <c r="DD19" s="17"/>
+      <c r="DE19" s="17"/>
+      <c r="DF19" s="17"/>
+      <c r="DG19" s="17"/>
+      <c r="DH19" s="17"/>
+      <c r="DI19" s="17"/>
+      <c r="DJ19" s="17"/>
+      <c r="DK19" s="17"/>
+      <c r="DL19" s="17"/>
+      <c r="DM19" s="17"/>
+      <c r="DN19" s="17"/>
+      <c r="DO19" s="17"/>
+      <c r="DP19" s="17"/>
+      <c r="DQ19" s="17"/>
+      <c r="DR19" s="17"/>
+      <c r="DS19" s="17"/>
+      <c r="DT19" s="17"/>
+      <c r="DU19" s="17"/>
+      <c r="DV19" s="17"/>
+      <c r="DW19" s="17"/>
+      <c r="DX19" s="17"/>
+      <c r="DY19" s="17"/>
+      <c r="DZ19" s="17"/>
+      <c r="EA19" s="17"/>
+      <c r="EB19" s="17"/>
+      <c r="EC19" s="17"/>
+      <c r="ED19" s="17"/>
+      <c r="EE19" s="17"/>
+      <c r="EF19" s="17"/>
+      <c r="EG19" s="17"/>
+      <c r="EH19" s="17"/>
+      <c r="EI19" s="17"/>
+      <c r="EJ19" s="17"/>
+      <c r="EK19" s="17"/>
+      <c r="EL19" s="17"/>
+      <c r="EM19" s="17"/>
+      <c r="EN19" s="17"/>
+      <c r="EO19" s="17"/>
+      <c r="EP19" s="17"/>
+      <c r="EQ19" s="17"/>
+      <c r="ER19" s="17"/>
+      <c r="ES19" s="17"/>
+      <c r="ET19" s="17"/>
+      <c r="EU19" s="17"/>
+      <c r="EV19" s="17"/>
+      <c r="EW19" s="17"/>
+      <c r="EX19" s="17"/>
+      <c r="EY19" s="17"/>
+      <c r="EZ19" s="17"/>
+      <c r="FA19" s="17"/>
+      <c r="FB19" s="17"/>
+      <c r="FC19" s="17"/>
+      <c r="FD19" s="17"/>
+      <c r="FE19" s="17"/>
+      <c r="FF19" s="17"/>
+      <c r="FG19" s="17"/>
+      <c r="FH19" s="17"/>
+      <c r="FI19" s="17"/>
+      <c r="FJ19" s="17"/>
+      <c r="FK19" s="17"/>
+      <c r="FL19" s="17"/>
+      <c r="FM19" s="17"/>
+      <c r="FN19" s="17"/>
+      <c r="FO19" s="17"/>
+      <c r="FP19" s="17"/>
+      <c r="FQ19" s="17"/>
+      <c r="FR19" s="17"/>
+      <c r="FS19" s="17"/>
+      <c r="FT19" s="17"/>
+      <c r="FU19" s="17"/>
+      <c r="FV19" s="17"/>
+      <c r="FW19" s="17"/>
+      <c r="FX19" s="17"/>
+      <c r="FY19" s="17"/>
+      <c r="FZ19" s="17"/>
+      <c r="GA19" s="17"/>
+      <c r="GB19" s="17"/>
+      <c r="GC19" s="17"/>
+      <c r="GD19" s="17"/>
+      <c r="GE19" s="17"/>
+      <c r="GF19" s="17"/>
+      <c r="GG19" s="17"/>
+      <c r="GH19" s="17"/>
+      <c r="GI19" s="17"/>
+      <c r="GJ19" s="17"/>
+      <c r="GK19" s="17"/>
+      <c r="GL19" s="17"/>
+      <c r="GM19" s="17"/>
+      <c r="GN19" s="17"/>
+      <c r="GO19" s="17"/>
+      <c r="GP19" s="17"/>
+      <c r="GQ19" s="17"/>
+      <c r="GR19" s="17"/>
+      <c r="GS19" s="17"/>
+      <c r="GT19" s="17"/>
+      <c r="GU19" s="17"/>
+      <c r="GV19" s="17"/>
+      <c r="GW19" s="17"/>
+      <c r="GX19" s="17"/>
+      <c r="GY19" s="17"/>
+      <c r="GZ19" s="17"/>
+      <c r="HA19" s="17"/>
+      <c r="HB19" s="17"/>
+      <c r="HC19" s="17"/>
+      <c r="HD19" s="17"/>
+      <c r="HE19" s="17"/>
+      <c r="HF19" s="17"/>
+      <c r="HG19" s="17"/>
+      <c r="HH19" s="17"/>
+      <c r="HI19" s="17"/>
+      <c r="HJ19" s="17"/>
+      <c r="HK19" s="17"/>
+      <c r="HL19" s="17"/>
+      <c r="HM19" s="17"/>
+      <c r="HN19" s="17"/>
+      <c r="HO19" s="17"/>
+      <c r="HP19" s="17"/>
+      <c r="HQ19" s="17"/>
+      <c r="HR19" s="17"/>
+      <c r="HS19" s="17"/>
+      <c r="HT19" s="17"/>
+      <c r="HU19" s="17"/>
+      <c r="HV19" s="17"/>
+      <c r="HW19" s="17"/>
+      <c r="HX19" s="17"/>
+      <c r="HY19" s="17"/>
+      <c r="HZ19" s="17"/>
+      <c r="IA19" s="17"/>
+      <c r="IB19" s="17"/>
+      <c r="IC19" s="17"/>
+      <c r="ID19" s="17"/>
+      <c r="IE19" s="17"/>
+      <c r="IF19" s="17"/>
+      <c r="IG19" s="17"/>
+      <c r="IH19" s="17"/>
+      <c r="II19" s="17"/>
+      <c r="IJ19" s="17"/>
+      <c r="IK19" s="17"/>
+      <c r="IL19" s="17"/>
+      <c r="IM19" s="17"/>
+      <c r="IN19" s="17"/>
+      <c r="IO19" s="17"/>
+      <c r="IP19" s="17"/>
+      <c r="IQ19" s="17"/>
+      <c r="IR19" s="17"/>
+      <c r="IS19" s="17"/>
+    </row>
+    <row r="20" spans="1:253" ht="32.25" customHeight="1">
+      <c r="A20" s="3">
+        <v>14</v>
+      </c>
+      <c r="B20" s="10">
+        <f t="shared" si="1"/>
+        <v>3255.84</v>
+      </c>
+      <c r="C20" s="10">
+        <f t="shared" si="0"/>
+        <v>3052.35</v>
+      </c>
+      <c r="D20" s="10">
+        <f t="shared" si="0"/>
+        <v>2872.7999999999997</v>
+      </c>
+      <c r="E20" s="10">
+        <f t="shared" si="0"/>
+        <v>2713.2</v>
+      </c>
+      <c r="F20" s="10">
+        <f t="shared" si="0"/>
+        <v>2570.4</v>
+      </c>
+      <c r="G20" s="11">
+        <f t="shared" si="0"/>
+        <v>2441.8799999999997</v>
+      </c>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="17"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="17"/>
+      <c r="W20" s="17"/>
+      <c r="X20" s="17"/>
+      <c r="Y20" s="17"/>
+      <c r="Z20" s="17"/>
+      <c r="AA20" s="17"/>
+      <c r="AB20" s="17"/>
+      <c r="AC20" s="17"/>
+      <c r="AD20" s="17"/>
+      <c r="AE20" s="17"/>
+      <c r="AF20" s="17"/>
+      <c r="AG20" s="17"/>
+      <c r="AH20" s="17"/>
+      <c r="AI20" s="17"/>
+      <c r="AJ20" s="17"/>
+      <c r="AK20" s="17"/>
+      <c r="AL20" s="17"/>
+      <c r="AM20" s="17"/>
+      <c r="AN20" s="17"/>
+      <c r="AO20" s="17"/>
+      <c r="AP20" s="17"/>
+      <c r="AQ20" s="17"/>
+      <c r="AR20" s="17"/>
+      <c r="AS20" s="17"/>
+      <c r="AT20" s="17"/>
+      <c r="AU20" s="17"/>
+      <c r="AV20" s="17"/>
+      <c r="AW20" s="17"/>
+      <c r="AX20" s="17"/>
+      <c r="AY20" s="17"/>
+      <c r="AZ20" s="17"/>
+      <c r="BA20" s="17"/>
+      <c r="BB20" s="17"/>
+      <c r="BC20" s="17"/>
+      <c r="BD20" s="17"/>
+      <c r="BE20" s="17"/>
+      <c r="BF20" s="17"/>
+      <c r="BG20" s="17"/>
+      <c r="BH20" s="17"/>
+      <c r="BI20" s="17"/>
+      <c r="BJ20" s="17"/>
+      <c r="BK20" s="17"/>
+      <c r="BL20" s="17"/>
+      <c r="BM20" s="17"/>
+      <c r="BN20" s="17"/>
+      <c r="BO20" s="17"/>
+      <c r="BP20" s="17"/>
+      <c r="BQ20" s="17"/>
+      <c r="BR20" s="17"/>
+      <c r="BS20" s="17"/>
+      <c r="BT20" s="17"/>
+      <c r="BU20" s="17"/>
+      <c r="BV20" s="17"/>
+      <c r="BW20" s="17"/>
+      <c r="BX20" s="17"/>
+      <c r="BY20" s="17"/>
+      <c r="BZ20" s="17"/>
+      <c r="CA20" s="17"/>
+      <c r="CB20" s="17"/>
+      <c r="CC20" s="17"/>
+      <c r="CD20" s="17"/>
+      <c r="CE20" s="17"/>
+      <c r="CF20" s="17"/>
+      <c r="CG20" s="17"/>
+      <c r="CH20" s="17"/>
+      <c r="CI20" s="17"/>
+      <c r="CJ20" s="17"/>
+      <c r="CK20" s="17"/>
+      <c r="CL20" s="17"/>
+      <c r="CM20" s="17"/>
+      <c r="CN20" s="17"/>
+      <c r="CO20" s="17"/>
+      <c r="CP20" s="17"/>
+      <c r="CQ20" s="17"/>
+      <c r="CR20" s="17"/>
+      <c r="CS20" s="17"/>
+      <c r="CT20" s="17"/>
+      <c r="CU20" s="17"/>
+      <c r="CV20" s="17"/>
+      <c r="CW20" s="17"/>
+      <c r="CX20" s="17"/>
+      <c r="CY20" s="17"/>
+      <c r="CZ20" s="17"/>
+      <c r="DA20" s="17"/>
+      <c r="DB20" s="17"/>
+      <c r="DC20" s="17"/>
+      <c r="DD20" s="17"/>
+      <c r="DE20" s="17"/>
+      <c r="DF20" s="17"/>
+      <c r="DG20" s="17"/>
+      <c r="DH20" s="17"/>
+      <c r="DI20" s="17"/>
+      <c r="DJ20" s="17"/>
+      <c r="DK20" s="17"/>
+      <c r="DL20" s="17"/>
+      <c r="DM20" s="17"/>
+      <c r="DN20" s="17"/>
+      <c r="DO20" s="17"/>
+      <c r="DP20" s="17"/>
+      <c r="DQ20" s="17"/>
+      <c r="DR20" s="17"/>
+      <c r="DS20" s="17"/>
+      <c r="DT20" s="17"/>
+      <c r="DU20" s="17"/>
+      <c r="DV20" s="17"/>
+      <c r="DW20" s="17"/>
+      <c r="DX20" s="17"/>
+      <c r="DY20" s="17"/>
+      <c r="DZ20" s="17"/>
+      <c r="EA20" s="17"/>
+      <c r="EB20" s="17"/>
+      <c r="EC20" s="17"/>
+      <c r="ED20" s="17"/>
+      <c r="EE20" s="17"/>
+      <c r="EF20" s="17"/>
+      <c r="EG20" s="17"/>
+      <c r="EH20" s="17"/>
+      <c r="EI20" s="17"/>
+      <c r="EJ20" s="17"/>
+      <c r="EK20" s="17"/>
+      <c r="EL20" s="17"/>
+      <c r="EM20" s="17"/>
+      <c r="EN20" s="17"/>
+      <c r="EO20" s="17"/>
+      <c r="EP20" s="17"/>
+      <c r="EQ20" s="17"/>
+      <c r="ER20" s="17"/>
+      <c r="ES20" s="17"/>
+      <c r="ET20" s="17"/>
+      <c r="EU20" s="17"/>
+      <c r="EV20" s="17"/>
+      <c r="EW20" s="17"/>
+      <c r="EX20" s="17"/>
+      <c r="EY20" s="17"/>
+      <c r="EZ20" s="17"/>
+      <c r="FA20" s="17"/>
+      <c r="FB20" s="17"/>
+      <c r="FC20" s="17"/>
+      <c r="FD20" s="17"/>
+      <c r="FE20" s="17"/>
+      <c r="FF20" s="17"/>
+      <c r="FG20" s="17"/>
+      <c r="FH20" s="17"/>
+      <c r="FI20" s="17"/>
+      <c r="FJ20" s="17"/>
+      <c r="FK20" s="17"/>
+      <c r="FL20" s="17"/>
+      <c r="FM20" s="17"/>
+      <c r="FN20" s="17"/>
+      <c r="FO20" s="17"/>
+      <c r="FP20" s="17"/>
+      <c r="FQ20" s="17"/>
+      <c r="FR20" s="17"/>
+      <c r="FS20" s="17"/>
+      <c r="FT20" s="17"/>
+      <c r="FU20" s="17"/>
+      <c r="FV20" s="17"/>
+      <c r="FW20" s="17"/>
+      <c r="FX20" s="17"/>
+      <c r="FY20" s="17"/>
+      <c r="FZ20" s="17"/>
+      <c r="GA20" s="17"/>
+      <c r="GB20" s="17"/>
+      <c r="GC20" s="17"/>
+      <c r="GD20" s="17"/>
+      <c r="GE20" s="17"/>
+      <c r="GF20" s="17"/>
+      <c r="GG20" s="17"/>
+      <c r="GH20" s="17"/>
+      <c r="GI20" s="17"/>
+      <c r="GJ20" s="17"/>
+      <c r="GK20" s="17"/>
+      <c r="GL20" s="17"/>
+      <c r="GM20" s="17"/>
+      <c r="GN20" s="17"/>
+      <c r="GO20" s="17"/>
+      <c r="GP20" s="17"/>
+      <c r="GQ20" s="17"/>
+      <c r="GR20" s="17"/>
+      <c r="GS20" s="17"/>
+      <c r="GT20" s="17"/>
+      <c r="GU20" s="17"/>
+      <c r="GV20" s="17"/>
+      <c r="GW20" s="17"/>
+      <c r="GX20" s="17"/>
+      <c r="GY20" s="17"/>
+      <c r="GZ20" s="17"/>
+      <c r="HA20" s="17"/>
+      <c r="HB20" s="17"/>
+      <c r="HC20" s="17"/>
+      <c r="HD20" s="17"/>
+      <c r="HE20" s="17"/>
+      <c r="HF20" s="17"/>
+      <c r="HG20" s="17"/>
+      <c r="HH20" s="17"/>
+      <c r="HI20" s="17"/>
+      <c r="HJ20" s="17"/>
+      <c r="HK20" s="17"/>
+      <c r="HL20" s="17"/>
+      <c r="HM20" s="17"/>
+      <c r="HN20" s="17"/>
+      <c r="HO20" s="17"/>
+      <c r="HP20" s="17"/>
+      <c r="HQ20" s="17"/>
+      <c r="HR20" s="17"/>
+      <c r="HS20" s="17"/>
+      <c r="HT20" s="17"/>
+      <c r="HU20" s="17"/>
+      <c r="HV20" s="17"/>
+      <c r="HW20" s="17"/>
+      <c r="HX20" s="17"/>
+      <c r="HY20" s="17"/>
+      <c r="HZ20" s="17"/>
+      <c r="IA20" s="17"/>
+      <c r="IB20" s="17"/>
+      <c r="IC20" s="17"/>
+      <c r="ID20" s="17"/>
+      <c r="IE20" s="17"/>
+      <c r="IF20" s="17"/>
+      <c r="IG20" s="17"/>
+      <c r="IH20" s="17"/>
+      <c r="II20" s="17"/>
+      <c r="IJ20" s="17"/>
+      <c r="IK20" s="17"/>
+      <c r="IL20" s="17"/>
+      <c r="IM20" s="17"/>
+      <c r="IN20" s="17"/>
+      <c r="IO20" s="17"/>
+      <c r="IP20" s="17"/>
+      <c r="IQ20" s="17"/>
+      <c r="IR20" s="17"/>
+      <c r="IS20" s="17"/>
+    </row>
+    <row r="21" spans="1:253" ht="32.25" customHeight="1">
+      <c r="A21" s="3">
+        <v>15</v>
+      </c>
+      <c r="B21" s="10">
+        <f t="shared" si="1"/>
+        <v>3270.375</v>
+      </c>
+      <c r="C21" s="10">
+        <f t="shared" si="0"/>
+        <v>3078</v>
+      </c>
+      <c r="D21" s="10">
+        <f t="shared" si="0"/>
+        <v>2907</v>
+      </c>
+      <c r="E21" s="10">
+        <f t="shared" si="0"/>
+        <v>2753.9999999999995</v>
+      </c>
+      <c r="F21" s="10">
+        <f t="shared" si="0"/>
+        <v>2616.2999999999997</v>
+      </c>
+      <c r="G21" s="11">
+        <f t="shared" si="0"/>
+        <v>2491.7142857142858</v>
+      </c>
+    </row>
+    <row r="23" spans="1:253" ht="30" customHeight="1">
+      <c r="A23" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B23" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
     </row>
-    <row r="18" spans="1:6" ht="18" customHeight="1">
-      <c r="A18" s="1" t="s">
+    <row r="24" spans="1:253" ht="18" customHeight="1">
+      <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B24" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
     </row>
-    <row r="19" spans="1:6" ht="18" customHeight="1">
-      <c r="A19" s="2" t="s">
+    <row r="25" spans="1:253" ht="18" customHeight="1">
+      <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B25" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
     </row>
-    <row r="20" spans="1:6" ht="18" customHeight="1">
-      <c r="B20" s="22" t="s">
+    <row r="26" spans="1:253" ht="18" customHeight="1">
+      <c r="B26" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
     </row>
-    <row r="21" spans="1:6" ht="18" customHeight="1">
-      <c r="B21" s="22" t="s">
+    <row r="27" spans="1:253" ht="18" customHeight="1">
+      <c r="B27" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
     </row>
-    <row r="23" spans="1:6" ht="18" customHeight="1">
-      <c r="B23" s="20" t="s">
+    <row r="29" spans="1:253" ht="18" customHeight="1">
+      <c r="B29" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
     </row>
-    <row r="24" spans="1:6" ht="18" customHeight="1">
-      <c r="B24" s="19" t="s">
+    <row r="30" spans="1:253" ht="18" customHeight="1">
+      <c r="B30" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
     </row>
-    <row r="25" spans="1:6" ht="41" customHeight="1">
-      <c r="B25" s="21" t="s">
+    <row r="31" spans="1:253" ht="41" customHeight="1">
+      <c r="B31" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
     </row>
-    <row r="27" spans="1:6" ht="41" customHeight="1">
-      <c r="B27" s="19" t="s">
+    <row r="32" spans="1:253" ht="41" customHeight="1">
+      <c r="B32" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
     </row>
-    <row r="29" spans="1:6" ht="33" customHeight="1">
-      <c r="B29" s="19" t="s">
+    <row r="34" spans="2:7" ht="33" customHeight="1">
+      <c r="B34" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B27:G27"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Added based updates for Jewel upgrade
</commit_message>
<xml_diff>
--- a/cookbooks/chef-bcs/files/default/utilities/BCS-Erasure-Coding-Calcs.xlsx
+++ b/cookbooks/chef-bcs/files/default/utilities/BCS-Erasure-Coding-Calcs.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27417"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisjones/projects/iqstack/chef-bcs/cookbooks/chef-bcs/files/default/utilities/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="0" windowWidth="21760" windowHeight="20460"/>
+    <workbookView xWindow="3640" yWindow="460" windowWidth="21760" windowHeight="20460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,9 +33,6 @@
   </si>
   <si>
     <t>Black - Calculated values</t>
-  </si>
-  <si>
-    <t>Bloomberg Cloud Storage (BCS) Erasure Coding Calculations</t>
   </si>
   <si>
     <t>M</t>
@@ -101,6 +106,9 @@
   <si>
     <t>*Storage Overhead - Approximate drive (HDD) overhead ratio from OS and misc</t>
   </si>
+  <si>
+    <t>Ceph Cloud Storage Erasure Coding Calculations</t>
+  </si>
 </sst>
 </file>
 
@@ -109,7 +117,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -603,6 +611,18 @@
     <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -627,9 +647,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -639,17 +656,8 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="64">
@@ -788,6 +796,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2042,10 +2055,10 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" sqref="A1:G1"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" customWidth="1"/>
@@ -2056,50 +2069,50 @@
     <col min="8" max="253" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:253" ht="36" customHeight="1">
-      <c r="A1" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+    <row r="1" spans="1:253" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
-    <row r="2" spans="1:253" ht="21" customHeight="1">
+    <row r="2" spans="1:253" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="19">
-        <v>612</v>
+        <v>1224</v>
       </c>
       <c r="C2" s="17"/>
-      <c r="D2" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="32"/>
+      <c r="D2" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="35"/>
       <c r="F2" s="22">
         <f>+B2*B5</f>
-        <v>3672</v>
+        <v>9792</v>
       </c>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:253" ht="21" customHeight="1">
+    <row r="3" spans="1:253" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="24">
+        <v>9.0700000000000003E-2</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="36">
-        <v>9.0700000000000003E-2</v>
-      </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="33"/>
+      <c r="E3" s="36"/>
       <c r="F3" s="18">
         <f>INT(+F2*0.0907)</f>
-        <v>333</v>
+        <v>888</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="11"/>
@@ -2349,21 +2362,21 @@
       <c r="IR3" s="11"/>
       <c r="IS3" s="11"/>
     </row>
-    <row r="4" spans="1:253" ht="20" customHeight="1">
+    <row r="4" spans="1:253" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="20">
         <v>0.95</v>
       </c>
       <c r="C4" s="17"/>
-      <c r="D4" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="38">
+      <c r="D4" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="38"/>
+      <c r="F4" s="25">
         <f>INT(+F2-F3*(1-B4))</f>
-        <v>3655</v>
+        <v>9747</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="9"/>
@@ -2613,40 +2626,40 @@
       <c r="IR4" s="9"/>
       <c r="IS4" s="9"/>
     </row>
-    <row r="5" spans="1:253" ht="20" customHeight="1">
+    <row r="5" spans="1:253" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="21">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5" s="17"/>
-      <c r="D5" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="35">
+      <c r="D5" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="37"/>
+      <c r="F5" s="23">
         <f>+F4-F3</f>
-        <v>3322</v>
+        <v>8859</v>
       </c>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:253" ht="20.5" customHeight="1">
+    <row r="6" spans="1:253" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33"/>
+    </row>
+    <row r="7" spans="1:253" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="29"/>
-    </row>
-    <row r="7" spans="1:253" ht="28" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="B7" s="12">
         <v>1</v>
@@ -2667,294 +2680,294 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:253" ht="28" customHeight="1">
+    <row r="8" spans="1:253" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>1</v>
       </c>
       <c r="B8" s="14">
         <f>+($B$2*$A8/($A8+B$7))*($B$5*(1-$B$3))*$B$4</f>
-        <v>1586.0010599999998</v>
+        <v>4229.3361599999998</v>
       </c>
       <c r="C8" s="14">
         <f t="shared" ref="C8:G22" si="0">+($B$2*$A8/($A8+C$7))*($B$5*(1-$B$3))*$B$4</f>
-        <v>1057.33404</v>
+        <v>2819.5574399999996</v>
       </c>
       <c r="D8" s="14">
         <f t="shared" si="0"/>
-        <v>793.00052999999991</v>
+        <v>2114.6680799999999</v>
       </c>
       <c r="E8" s="14">
         <f t="shared" si="0"/>
-        <v>634.40042400000004</v>
+        <v>1691.7344639999999</v>
       </c>
       <c r="F8" s="14">
         <f t="shared" si="0"/>
-        <v>528.66701999999998</v>
+        <v>1409.7787199999998</v>
       </c>
       <c r="G8" s="15">
         <f t="shared" si="0"/>
-        <v>453.14315999999997</v>
+        <v>1208.38176</v>
       </c>
     </row>
-    <row r="9" spans="1:253" ht="32" customHeight="1">
+    <row r="9" spans="1:253" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>2</v>
       </c>
       <c r="B9" s="14">
-        <f t="shared" ref="B9:G22" si="1">+($B$2*$A9/($A9+B$7))*($B$5*(1-$B$3))*$B$4</f>
+        <f t="shared" ref="B9:B22" si="1">+($B$2*$A9/($A9+B$7))*($B$5*(1-$B$3))*$B$4</f>
+        <v>5639.1148799999992</v>
+      </c>
+      <c r="C9" s="14">
+        <f t="shared" si="0"/>
+        <v>4229.3361599999998</v>
+      </c>
+      <c r="D9" s="14">
+        <f t="shared" si="0"/>
+        <v>3383.4689279999998</v>
+      </c>
+      <c r="E9" s="14">
+        <f t="shared" si="0"/>
+        <v>2819.5574399999996</v>
+      </c>
+      <c r="F9" s="14">
+        <f t="shared" si="0"/>
+        <v>2416.76352</v>
+      </c>
+      <c r="G9" s="15">
+        <f t="shared" si="0"/>
         <v>2114.6680799999999</v>
       </c>
-      <c r="C9" s="14">
-        <f t="shared" si="0"/>
-        <v>1586.0010599999998</v>
-      </c>
-      <c r="D9" s="14">
-        <f t="shared" si="0"/>
-        <v>1268.8008480000001</v>
-      </c>
-      <c r="E9" s="14">
-        <f t="shared" si="0"/>
-        <v>1057.33404</v>
-      </c>
-      <c r="F9" s="14">
-        <f t="shared" si="0"/>
-        <v>906.28631999999993</v>
-      </c>
-      <c r="G9" s="15">
-        <f t="shared" si="0"/>
-        <v>793.00052999999991</v>
-      </c>
     </row>
-    <row r="10" spans="1:253" ht="31" customHeight="1">
+    <row r="10" spans="1:253" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>3</v>
       </c>
       <c r="B10" s="14">
         <f t="shared" si="1"/>
-        <v>2379.0015899999999</v>
+        <v>6344.0042399999993</v>
       </c>
       <c r="C10" s="14">
         <f t="shared" si="0"/>
-        <v>1903.201272</v>
+        <v>5075.2033919999994</v>
       </c>
       <c r="D10" s="14">
         <f t="shared" si="0"/>
-        <v>1586.0010599999998</v>
+        <v>4229.3361599999998</v>
       </c>
       <c r="E10" s="14">
         <f t="shared" si="0"/>
-        <v>1359.42948</v>
+        <v>3625.1452799999997</v>
       </c>
       <c r="F10" s="14">
         <f t="shared" si="0"/>
-        <v>1189.5007949999999</v>
+        <v>3172.0021199999996</v>
       </c>
       <c r="G10" s="15">
         <f t="shared" si="0"/>
-        <v>1057.33404</v>
+        <v>2819.5574399999996</v>
       </c>
     </row>
-    <row r="11" spans="1:253" ht="32.25" customHeight="1">
+    <row r="11" spans="1:253" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>4</v>
       </c>
       <c r="B11" s="14">
         <f t="shared" si="1"/>
-        <v>2537.6016960000002</v>
+        <v>6766.9378559999996</v>
       </c>
       <c r="C11" s="14">
         <f t="shared" si="0"/>
-        <v>2114.6680799999999</v>
+        <v>5639.1148799999992</v>
       </c>
       <c r="D11" s="14">
         <f t="shared" si="0"/>
-        <v>1812.5726399999999</v>
+        <v>4833.5270399999999</v>
       </c>
       <c r="E11" s="14">
         <f t="shared" si="0"/>
-        <v>1586.0010599999998</v>
+        <v>4229.3361599999998</v>
       </c>
       <c r="F11" s="14">
         <f t="shared" si="0"/>
-        <v>1409.7787199999998</v>
+        <v>3759.4099199999996</v>
       </c>
       <c r="G11" s="15">
         <f t="shared" si="0"/>
-        <v>1268.8008480000001</v>
+        <v>3383.4689279999998</v>
       </c>
     </row>
-    <row r="12" spans="1:253" ht="32.25" customHeight="1">
+    <row r="12" spans="1:253" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>5</v>
       </c>
       <c r="B12" s="14">
         <f t="shared" si="1"/>
-        <v>2643.3350999999998</v>
+        <v>7048.8935999999994</v>
       </c>
       <c r="C12" s="14">
         <f t="shared" si="0"/>
-        <v>2265.7157999999999</v>
+        <v>6041.9088000000002</v>
       </c>
       <c r="D12" s="14">
         <f t="shared" si="0"/>
-        <v>1982.501325</v>
+        <v>5286.6701999999996</v>
       </c>
       <c r="E12" s="14">
         <f t="shared" si="0"/>
-        <v>1762.2233999999999</v>
+        <v>4699.2623999999996</v>
       </c>
       <c r="F12" s="14">
         <f t="shared" si="0"/>
-        <v>1586.0010599999998</v>
+        <v>4229.3361599999998</v>
       </c>
       <c r="G12" s="15">
         <f t="shared" si="0"/>
-        <v>1441.8191454545454</v>
+        <v>3844.8510545454546</v>
       </c>
     </row>
-    <row r="13" spans="1:253" ht="32.25" customHeight="1">
+    <row r="13" spans="1:253" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>6</v>
       </c>
       <c r="B13" s="14">
         <f t="shared" si="1"/>
-        <v>2718.85896</v>
+        <v>7250.2905599999995</v>
       </c>
       <c r="C13" s="14">
         <f t="shared" si="0"/>
-        <v>2379.0015899999999</v>
+        <v>6344.0042399999993</v>
       </c>
       <c r="D13" s="14">
         <f t="shared" si="0"/>
-        <v>2114.6680799999999</v>
+        <v>5639.1148799999992</v>
       </c>
       <c r="E13" s="14">
         <f t="shared" si="0"/>
-        <v>1903.201272</v>
+        <v>5075.2033919999994</v>
       </c>
       <c r="F13" s="14">
         <f t="shared" si="0"/>
-        <v>1730.1829745454545</v>
+        <v>4613.821265454545</v>
       </c>
       <c r="G13" s="15">
         <f t="shared" si="0"/>
-        <v>1586.0010599999998</v>
+        <v>4229.3361599999998</v>
       </c>
     </row>
-    <row r="14" spans="1:253" ht="32.25" customHeight="1">
+    <row r="14" spans="1:253" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>7</v>
       </c>
       <c r="B14" s="14">
         <f t="shared" si="1"/>
-        <v>2775.501855</v>
+        <v>7401.3382799999999</v>
       </c>
       <c r="C14" s="14">
         <f t="shared" si="0"/>
-        <v>2467.1127599999995</v>
+        <v>6578.9673599999996</v>
       </c>
       <c r="D14" s="14">
         <f t="shared" si="0"/>
-        <v>2220.4014839999995</v>
+        <v>5921.070623999999</v>
       </c>
       <c r="E14" s="14">
         <f t="shared" si="0"/>
-        <v>2018.5468036363636</v>
+        <v>5382.7914763636354</v>
       </c>
       <c r="F14" s="14">
         <f t="shared" si="0"/>
-        <v>1850.33457</v>
+        <v>4934.2255199999991</v>
       </c>
       <c r="G14" s="15">
         <f t="shared" si="0"/>
-        <v>1708.0011415384615</v>
+        <v>4554.6697107692307</v>
       </c>
     </row>
-    <row r="15" spans="1:253" ht="32.25" customHeight="1">
+    <row r="15" spans="1:253" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>8</v>
       </c>
       <c r="B15" s="14">
         <f t="shared" si="1"/>
-        <v>2819.5574399999996</v>
+        <v>7518.8198399999992</v>
       </c>
       <c r="C15" s="14">
         <f t="shared" si="0"/>
-        <v>2537.6016960000002</v>
+        <v>6766.9378559999996</v>
       </c>
       <c r="D15" s="14">
         <f t="shared" si="0"/>
-        <v>2306.9106327272725</v>
+        <v>6151.7616872727267</v>
       </c>
       <c r="E15" s="14">
         <f t="shared" si="0"/>
-        <v>2114.6680799999999</v>
+        <v>5639.1148799999992</v>
       </c>
       <c r="F15" s="14">
         <f t="shared" si="0"/>
-        <v>1952.0013046153847</v>
+        <v>5205.3368123076925</v>
       </c>
       <c r="G15" s="15">
         <f t="shared" si="0"/>
-        <v>1812.5726399999999</v>
+        <v>4833.5270399999999</v>
       </c>
     </row>
-    <row r="16" spans="1:253" ht="32.25" customHeight="1">
+    <row r="16" spans="1:253" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>9</v>
       </c>
       <c r="B16" s="14">
         <f t="shared" si="1"/>
-        <v>2854.8019079999999</v>
+        <v>7612.8050879999992</v>
       </c>
       <c r="C16" s="14">
         <f t="shared" si="0"/>
-        <v>2595.2744618181819</v>
+        <v>6920.731898181818</v>
       </c>
       <c r="D16" s="14">
         <f t="shared" si="0"/>
-        <v>2379.0015899999999</v>
+        <v>6344.0042399999993</v>
       </c>
       <c r="E16" s="14">
         <f t="shared" si="0"/>
-        <v>2196.0014676923074</v>
+        <v>5856.0039138461534</v>
       </c>
       <c r="F16" s="14">
         <f t="shared" si="0"/>
-        <v>2039.1442199999999</v>
+        <v>5437.71792</v>
       </c>
       <c r="G16" s="15">
         <f t="shared" si="0"/>
-        <v>1903.201272</v>
+        <v>5075.2033919999994</v>
       </c>
     </row>
-    <row r="17" spans="1:253" ht="32.25" customHeight="1">
+    <row r="17" spans="1:253" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>10</v>
       </c>
       <c r="B17" s="14">
         <f t="shared" si="1"/>
-        <v>2883.6382909090908</v>
+        <v>7689.7021090909093</v>
       </c>
       <c r="C17" s="14">
         <f t="shared" si="0"/>
-        <v>2643.3350999999998</v>
+        <v>7048.8935999999994</v>
       </c>
       <c r="D17" s="14">
         <f t="shared" si="0"/>
-        <v>2440.0016307692304</v>
+        <v>6506.6710153846152</v>
       </c>
       <c r="E17" s="14">
         <f t="shared" si="0"/>
-        <v>2265.7157999999999</v>
+        <v>6041.9088000000002</v>
       </c>
       <c r="F17" s="14">
         <f t="shared" si="0"/>
-        <v>2114.6680799999999</v>
+        <v>5639.1148799999992</v>
       </c>
       <c r="G17" s="15">
         <f t="shared" si="0"/>
-        <v>1982.501325</v>
+        <v>5286.6701999999996</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -3203,33 +3216,33 @@
       <c r="IR17" s="6"/>
       <c r="IS17" s="6"/>
     </row>
-    <row r="18" spans="1:253" ht="32.25" customHeight="1">
+    <row r="18" spans="1:253" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>11</v>
       </c>
       <c r="B18" s="14">
         <f t="shared" si="1"/>
-        <v>2907.6686099999997</v>
+        <v>7753.7829599999995</v>
       </c>
       <c r="C18" s="14">
         <f t="shared" si="0"/>
-        <v>2684.0017938461538</v>
+        <v>7157.3381169230761</v>
       </c>
       <c r="D18" s="14">
         <f t="shared" si="0"/>
-        <v>2492.2873799999998</v>
+        <v>6646.0996799999994</v>
       </c>
       <c r="E18" s="14">
         <f t="shared" si="0"/>
-        <v>2326.134888</v>
+        <v>6203.0263679999998</v>
       </c>
       <c r="F18" s="14">
         <f t="shared" si="0"/>
-        <v>2180.7514575</v>
+        <v>5815.3372199999994</v>
       </c>
       <c r="G18" s="15">
         <f t="shared" si="0"/>
-        <v>2052.4719599999999</v>
+        <v>5473.2585600000002</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -3478,33 +3491,33 @@
       <c r="IR18" s="6"/>
       <c r="IS18" s="6"/>
     </row>
-    <row r="19" spans="1:253" ht="32.25" customHeight="1">
+    <row r="19" spans="1:253" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>12</v>
       </c>
       <c r="B19" s="14">
         <f t="shared" si="1"/>
-        <v>2928.0019569230767</v>
+        <v>7808.005218461537</v>
       </c>
       <c r="C19" s="14">
         <f t="shared" si="0"/>
-        <v>2718.85896</v>
+        <v>7250.2905599999995</v>
       </c>
       <c r="D19" s="14">
         <f t="shared" si="0"/>
-        <v>2537.6016960000002</v>
+        <v>6766.9378559999996</v>
       </c>
       <c r="E19" s="14">
         <f t="shared" si="0"/>
-        <v>2379.0015899999999</v>
+        <v>6344.0042399999993</v>
       </c>
       <c r="F19" s="14">
         <f t="shared" si="0"/>
-        <v>2239.06032</v>
+        <v>5970.8275199999989</v>
       </c>
       <c r="G19" s="15">
         <f t="shared" si="0"/>
-        <v>2114.6680799999999</v>
+        <v>5639.1148799999992</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -3753,33 +3766,33 @@
       <c r="IR19" s="6"/>
       <c r="IS19" s="6"/>
     </row>
-    <row r="20" spans="1:253" ht="32.25" customHeight="1">
+    <row r="20" spans="1:253" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>13</v>
       </c>
       <c r="B20" s="14">
         <f t="shared" si="1"/>
-        <v>2945.4305400000003</v>
+        <v>7854.4814399999996</v>
       </c>
       <c r="C20" s="14">
         <f t="shared" si="0"/>
-        <v>2749.0685039999998</v>
+        <v>7330.8493439999993</v>
       </c>
       <c r="D20" s="14">
         <f t="shared" si="0"/>
-        <v>2577.2517224999997</v>
+        <v>6872.6712600000001</v>
       </c>
       <c r="E20" s="14">
         <f t="shared" si="0"/>
-        <v>2425.6486800000002</v>
+        <v>6468.3964799999994</v>
       </c>
       <c r="F20" s="14">
         <f t="shared" si="0"/>
-        <v>2290.8904199999997</v>
+        <v>6109.0411199999999</v>
       </c>
       <c r="G20" s="15">
         <f t="shared" si="0"/>
-        <v>2170.3172399999999</v>
+        <v>5787.5126399999999</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -4028,33 +4041,33 @@
       <c r="IR20" s="6"/>
       <c r="IS20" s="6"/>
     </row>
-    <row r="21" spans="1:253" ht="32.25" customHeight="1">
+    <row r="21" spans="1:253" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>14</v>
       </c>
       <c r="B21" s="14">
         <f t="shared" si="1"/>
-        <v>2960.535312</v>
+        <v>7894.760831999999</v>
       </c>
       <c r="C21" s="14">
         <f t="shared" si="0"/>
-        <v>2775.501855</v>
+        <v>7401.3382799999999</v>
       </c>
       <c r="D21" s="14">
         <f t="shared" si="0"/>
-        <v>2612.23704</v>
+        <v>6965.965439999999</v>
       </c>
       <c r="E21" s="14">
         <f t="shared" si="0"/>
-        <v>2467.1127599999995</v>
+        <v>6578.9673599999996</v>
       </c>
       <c r="F21" s="14">
         <f t="shared" si="0"/>
-        <v>2337.2647200000001</v>
+        <v>6232.7059199999994</v>
       </c>
       <c r="G21" s="15">
         <f t="shared" si="0"/>
-        <v>2220.4014839999995</v>
+        <v>5921.070623999999</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
@@ -4303,58 +4316,58 @@
       <c r="IR21" s="6"/>
       <c r="IS21" s="6"/>
     </row>
-    <row r="22" spans="1:253" ht="32.25" customHeight="1">
+    <row r="22" spans="1:253" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>15</v>
       </c>
       <c r="B22" s="14">
         <f t="shared" si="1"/>
-        <v>2973.7519874999998</v>
+        <v>7930.0052999999998</v>
       </c>
       <c r="C22" s="14">
         <f t="shared" si="0"/>
-        <v>2798.8253999999997</v>
+        <v>7463.5343999999996</v>
       </c>
       <c r="D22" s="14">
         <f t="shared" si="0"/>
-        <v>2643.3350999999998</v>
+        <v>7048.8935999999994</v>
       </c>
       <c r="E22" s="14">
         <f t="shared" si="0"/>
-        <v>2504.2121999999999</v>
+        <v>6677.8991999999998</v>
       </c>
       <c r="F22" s="14">
         <f t="shared" si="0"/>
-        <v>2379.0015899999999</v>
+        <v>6344.0042399999993</v>
       </c>
       <c r="G22" s="15">
         <f t="shared" si="0"/>
-        <v>2265.7157999999999</v>
+        <v>6041.9088000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:253" ht="30" customHeight="1">
+    <row r="24" spans="1:253" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
+      <c r="B24" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
     </row>
-    <row r="25" spans="1:253" ht="21" customHeight="1">
+    <row r="25" spans="1:253" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
-      <c r="B25" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
+      <c r="B25" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
@@ -4602,114 +4615,116 @@
       <c r="IR25" s="11"/>
       <c r="IS25" s="11"/>
     </row>
-    <row r="26" spans="1:253" ht="18" customHeight="1">
+    <row r="26" spans="1:253" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+    </row>
+    <row r="27" spans="1:253" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
     </row>
-    <row r="27" spans="1:253" ht="18" customHeight="1">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:253" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+    </row>
+    <row r="29" spans="1:253" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+    </row>
+    <row r="31" spans="1:253" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+    </row>
+    <row r="32" spans="1:253" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+    </row>
+    <row r="33" spans="2:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
     </row>
-    <row r="28" spans="1:253" ht="18" customHeight="1">
-      <c r="B28" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
+    <row r="34" spans="2:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
     </row>
-    <row r="29" spans="1:253" ht="18" customHeight="1">
-      <c r="B29" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
+    <row r="35" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
     </row>
-    <row r="31" spans="1:253" ht="18" customHeight="1">
-      <c r="B31" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-    </row>
-    <row r="32" spans="1:253" ht="18" customHeight="1">
-      <c r="B32" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-    </row>
-    <row r="33" spans="2:7" ht="41" customHeight="1">
-      <c r="B33" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-    </row>
-    <row r="34" spans="2:7" ht="41" customHeight="1">
-      <c r="B34" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-    </row>
-    <row r="35" spans="2:7" ht="33" customHeight="1">
-      <c r="B35" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-    </row>
-    <row r="36" spans="2:7" ht="27" customHeight="1">
-      <c r="B36" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
+    <row r="36" spans="2:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D4:E4"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B35:G35"/>
@@ -4726,18 +4741,11 @@
     <mergeCell ref="B29:G29"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>